<commit_message>
10/05 18시 56분 negative part
</commit_message>
<xml_diff>
--- a/datasets/oneword_concat.xlsx
+++ b/datasets/oneword_concat.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>one_char_keyword</t>
   </si>
@@ -62,12 +62,6 @@
   </si>
   <si>
     <t>맵</t>
-  </si>
-  <si>
-    <t>몇</t>
-  </si>
-  <si>
-    <t>못</t>
   </si>
   <si>
     <t>물</t>
@@ -696,74 +690,70 @@
       <c r="C17" s="5"/>
     </row>
     <row r="18" ht="18.0" customHeight="1">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="6"/>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" ht="18.0" customHeight="1">
+      <c r="A19" s="6"/>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" ht="18.0" customHeight="1">
+      <c r="A20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" ht="18.0" customHeight="1">
-      <c r="A19" s="6" t="s">
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" ht="18.0" customHeight="1">
+      <c r="A21" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" ht="18.0" customHeight="1">
-      <c r="A20" s="8" t="s">
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" ht="18.0" customHeight="1">
+      <c r="A22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" ht="18.0" customHeight="1">
-      <c r="A21" s="6" t="s">
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" ht="18.0" customHeight="1">
+      <c r="A23" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" ht="18.0" customHeight="1">
-      <c r="A22" s="8" t="s">
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" ht="18.0" customHeight="1">
+      <c r="A24" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" ht="18.0" customHeight="1">
-      <c r="A23" s="6" t="s">
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" ht="18.0" customHeight="1">
+      <c r="A25" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" ht="18.0" customHeight="1">
-      <c r="A24" s="6" t="s">
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" ht="18.0" customHeight="1">
+      <c r="A26" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" ht="18.0" customHeight="1">
-      <c r="A25" s="6" t="s">
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" ht="18.0" customHeight="1">
+      <c r="A27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" ht="18.0" customHeight="1">
-      <c r="A26" s="6" t="s">
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" ht="18.0" customHeight="1">
+      <c r="A28" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" ht="18.0" customHeight="1">
-      <c r="A27" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="5"/>
-    </row>
-    <row r="28" ht="18.0" customHeight="1">
-      <c r="A28" s="6" t="s">
-        <v>27</v>
-      </c>
       <c r="C28" s="5"/>
     </row>
     <row r="29" ht="18.0" customHeight="1">
       <c r="A29" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C29" s="5"/>
     </row>
@@ -773,193 +763,193 @@
     </row>
     <row r="31" ht="18.0" customHeight="1">
       <c r="A31" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" ht="18.0" customHeight="1">
+      <c r="A32" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" ht="18.0" customHeight="1">
+      <c r="A33" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="5"/>
-    </row>
-    <row r="32" ht="18.0" customHeight="1">
-      <c r="A32" s="6" t="s">
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" ht="18.0" customHeight="1">
+      <c r="A34" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" ht="18.0" customHeight="1">
-      <c r="A33" s="6" t="s">
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" ht="18.0" customHeight="1">
+      <c r="A35" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="5"/>
-    </row>
-    <row r="34" ht="18.0" customHeight="1">
-      <c r="A34" s="6" t="s">
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" ht="18.0" customHeight="1">
+      <c r="A36" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="5"/>
-    </row>
-    <row r="35" ht="18.0" customHeight="1">
-      <c r="A35" s="6" t="s">
+      <c r="C36" s="5"/>
+    </row>
+    <row r="37" ht="18.0" customHeight="1">
+      <c r="A37" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="5"/>
-    </row>
-    <row r="36" ht="18.0" customHeight="1">
-      <c r="A36" s="6" t="s">
+      <c r="C37" s="5"/>
+    </row>
+    <row r="38" ht="18.0" customHeight="1">
+      <c r="A38" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="5"/>
-    </row>
-    <row r="37" ht="18.0" customHeight="1">
-      <c r="A37" s="6" t="s">
+      <c r="C38" s="5"/>
+    </row>
+    <row r="39" ht="18.0" customHeight="1">
+      <c r="A39" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="5"/>
-    </row>
-    <row r="38" ht="18.0" customHeight="1">
-      <c r="A38" s="9" t="s">
+      <c r="C39" s="5"/>
+    </row>
+    <row r="40" ht="18.0" customHeight="1">
+      <c r="A40" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="5"/>
-    </row>
-    <row r="39" ht="18.0" customHeight="1">
-      <c r="A39" s="6" t="s">
+      <c r="C40" s="5"/>
+    </row>
+    <row r="41" ht="18.0" customHeight="1">
+      <c r="A41" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="5"/>
-    </row>
-    <row r="40" ht="18.0" customHeight="1">
-      <c r="A40" s="6" t="s">
+      <c r="C41" s="5"/>
+    </row>
+    <row r="42" ht="18.0" customHeight="1">
+      <c r="A42" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="5"/>
-    </row>
-    <row r="41" ht="18.0" customHeight="1">
-      <c r="A41" s="6" t="s">
+      <c r="C42" s="5"/>
+    </row>
+    <row r="43" ht="18.0" customHeight="1">
+      <c r="A43" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="5"/>
-    </row>
-    <row r="42" ht="18.0" customHeight="1">
-      <c r="A42" s="6" t="s">
+      <c r="C43" s="5"/>
+    </row>
+    <row r="44" ht="18.0" customHeight="1">
+      <c r="A44" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="5"/>
-    </row>
-    <row r="43" ht="18.0" customHeight="1">
-      <c r="A43" s="6" t="s">
+      <c r="C44" s="5"/>
+    </row>
+    <row r="45" ht="18.0" customHeight="1">
+      <c r="A45" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="5"/>
-    </row>
-    <row r="44" ht="18.0" customHeight="1">
-      <c r="A44" s="6" t="s">
+      <c r="C45" s="5"/>
+    </row>
+    <row r="46" ht="18.0" customHeight="1">
+      <c r="A46" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="5"/>
-    </row>
-    <row r="45" ht="18.0" customHeight="1">
-      <c r="A45" s="6" t="s">
+      <c r="C46" s="5"/>
+    </row>
+    <row r="47" ht="18.0" customHeight="1">
+      <c r="A47" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="5"/>
-    </row>
-    <row r="46" ht="18.0" customHeight="1">
-      <c r="A46" s="6" t="s">
+      <c r="C47" s="5"/>
+    </row>
+    <row r="48" ht="18.0" customHeight="1">
+      <c r="A48" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="5"/>
-    </row>
-    <row r="47" ht="18.0" customHeight="1">
-      <c r="A47" s="6" t="s">
+      <c r="C48" s="5"/>
+    </row>
+    <row r="49" ht="18.0" customHeight="1">
+      <c r="A49" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="5"/>
-    </row>
-    <row r="48" ht="18.0" customHeight="1">
-      <c r="A48" s="6" t="s">
+      <c r="C49" s="5"/>
+    </row>
+    <row r="50" ht="18.0" customHeight="1">
+      <c r="A50" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="5"/>
-    </row>
-    <row r="49" ht="18.0" customHeight="1">
-      <c r="A49" s="8" t="s">
+      <c r="C50" s="5"/>
+    </row>
+    <row r="51" ht="18.0" customHeight="1">
+      <c r="A51" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="5"/>
-    </row>
-    <row r="50" ht="18.0" customHeight="1">
-      <c r="A50" s="6" t="s">
+      <c r="C51" s="5"/>
+    </row>
+    <row r="52" ht="18.0" customHeight="1">
+      <c r="A52" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="5"/>
-    </row>
-    <row r="51" ht="18.0" customHeight="1">
-      <c r="A51" s="6" t="s">
+      <c r="C52" s="5"/>
+    </row>
+    <row r="53" ht="18.0" customHeight="1">
+      <c r="A53" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="5"/>
-    </row>
-    <row r="52" ht="18.0" customHeight="1">
-      <c r="A52" s="6" t="s">
+      <c r="C53" s="5"/>
+    </row>
+    <row r="54" ht="18.0" customHeight="1">
+      <c r="A54" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C52" s="5"/>
-    </row>
-    <row r="53" ht="18.0" customHeight="1">
-      <c r="A53" s="6" t="s">
+      <c r="C54" s="5"/>
+    </row>
+    <row r="55" ht="18.0" customHeight="1">
+      <c r="A55" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C53" s="5"/>
-    </row>
-    <row r="54" ht="18.0" customHeight="1">
-      <c r="A54" s="6" t="s">
+      <c r="C55" s="5"/>
+    </row>
+    <row r="56" ht="18.0" customHeight="1">
+      <c r="A56" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C54" s="5"/>
-    </row>
-    <row r="55" ht="18.0" customHeight="1">
-      <c r="A55" s="6" t="s">
+      <c r="C56" s="5"/>
+    </row>
+    <row r="57" ht="18.0" customHeight="1">
+      <c r="A57" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C55" s="5"/>
-    </row>
-    <row r="56" ht="18.0" customHeight="1">
-      <c r="A56" s="6" t="s">
+      <c r="C57" s="5"/>
+    </row>
+    <row r="58" ht="18.0" customHeight="1">
+      <c r="A58" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C56" s="5"/>
-    </row>
-    <row r="57" ht="18.0" customHeight="1">
-      <c r="A57" s="6" t="s">
+      <c r="C58" s="5"/>
+    </row>
+    <row r="59" ht="18.0" customHeight="1">
+      <c r="A59" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C57" s="5"/>
-    </row>
-    <row r="58" ht="18.0" customHeight="1">
-      <c r="A58" s="6" t="s">
+      <c r="C59" s="5"/>
+    </row>
+    <row r="60" ht="18.0" customHeight="1">
+      <c r="A60" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C58" s="5"/>
-    </row>
-    <row r="59" ht="18.0" customHeight="1">
-      <c r="A59" s="6" t="s">
+      <c r="C60" s="5"/>
+    </row>
+    <row r="61" ht="18.0" customHeight="1">
+      <c r="A61" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C59" s="5"/>
-    </row>
-    <row r="60" ht="18.0" customHeight="1">
-      <c r="A60" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C60" s="5"/>
-    </row>
-    <row r="61" ht="18.0" customHeight="1">
-      <c r="A61" s="6" t="s">
-        <v>59</v>
-      </c>
       <c r="C61" s="5"/>
     </row>
     <row r="62" ht="18.0" customHeight="1">
       <c r="A62" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C62" s="5"/>
     </row>

</xml_diff>